<commit_message>
fix regex for microalbuminurie
</commit_message>
<xml_diff>
--- a/data/variable_biologique_bioLOINC.xlsx
+++ b/data/variable_biologique_bioLOINC.xlsx
@@ -9,11 +9,11 @@
     <sheet state="visible" name="extract" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="Z_0DB99419_9870_4585_B335_92597D4BBC61_.wvu.FilterData">CiblageProtocoleLOINC!$A$1:$AC$997</definedName>
+    <definedName hidden="1" localSheetId="1" name="Z_3E33EBCD_DBEA_4B3A_B55F_184CA4B5D9E5_.wvu.FilterData">CiblageProtocoleLOINC!$A$1:$AC$997</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0DB99419-9870-4585-B335-92597D4BBC61}" name="Filtre 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3E33EBCD-DBEA-4B3A-B55F-184CA4B5D9E5}" name="Filtre 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Albuminurie, Albumine (urines), Albumine urinaire, Albumin, Microalbuminurie</t>
   </si>
   <si>
-    <t>[aA]lbuminurie|([aA]lbumin.{1,10}[uU]rin[^ ]*)|[aA]lbumine[^ ]*</t>
+    <t>[aA]lbuminurie|([aA]lbumin.{1,10}[uU]rin[^ ]*)|([Mmicro]{5})?[aA]lbumi[^ ]*</t>
   </si>
   <si>
     <t>mg/L</t>
@@ -456,10 +456,10 @@
     <t>HbA1c</t>
   </si>
   <si>
-    <t>Hémoglobine glyquée, Hémoglobine glycosylée, HbA1c</t>
-  </si>
-  <si>
-    <t>H[bB]A1[cC]|([hH].moglobin.{1,4}[gG]l[iy]c[^ ]*)</t>
+    <t>Hémoglobine glyquée, Hémoglobine glycosylée, HbA1c, Hémoglobine A1c</t>
+  </si>
+  <si>
+    <t>H[bB]A1[cC]|([hH].moglobin.{1,4}[gG]l[iy]c[^ ]*)|[hH].moglobine [Aa]1[cC]</t>
   </si>
   <si>
     <t>%</t>
@@ -11820,7 +11820,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0DB99419-9870-4585-B335-92597D4BBC61}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{3E33EBCD-DBEA-4B3A-B55F-184CA4B5D9E5}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$AC$997"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>